<commit_message>
worked on cis17c final problem #3, bank queue.
Signed-off-by: koa2019 <no-reply>
</commit_message>
<xml_diff>
--- a/final/prb3_queue/prb3_queueBank_v1.xlsx
+++ b/final/prb3_queue/prb3_queueBank_v1.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanYell\Documents\cis17c_git2\final\prb3_queue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFA3D88-423D-4F08-B4AB-60B0CBEE72FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56772027-C0B9-4F02-A151-2A34F1E2AC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{ED522311-96CF-4CCA-A0CA-B46BB6F16CC7}"/>
   </bookViews>
   <sheets>
-    <sheet name="p3_que" sheetId="1" r:id="rId1"/>
+    <sheet name="p3_que_2" sheetId="1" r:id="rId1"/>
+    <sheet name="output" sheetId="2" r:id="rId2"/>
+    <sheet name="p3_que_1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>queue in back</t>
   </si>
@@ -117,13 +119,187 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>numInBank++</t>
+  </si>
+  <si>
+    <t>sum clerks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  60 nClerks=3 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  65 nClerks=3 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  70 nClerks=3 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  75 nClerks=3 nInBank=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  80 nClerks=3 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  85 nClerks=3 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  90 nClerks=3 nInBank=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  95 nClerks=3 nInBank=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 100 nClerks=3 nInBank=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 105 nClerks=3 nInBank=6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 110 nClerks=3 nInBank=6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 115 nClerks=3 nInBank=6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 120 nClerks=3 nInBank=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 125 nClerks=3 nInBank=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 130 nClerks=3 nInBank=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 135 nClerks=3 nInBank=6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 140 nClerks=3 nInBank=6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 145 nClerks=3 nInBank=6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 150 nClerks=3 nInBank=7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 155 nClerks=3 nInBank=7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 160 nClerks=3 nInBank=6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 165 nClerks=3 nInBank=7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 170 nClerks=3 nInBank=7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 175 nClerks=3 nInBank=7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 180 nClerks=3 nInBank=7</t>
+  </si>
+  <si>
+    <t>nClerks++</t>
+  </si>
+  <si>
+    <t>nClerks = 3</t>
+  </si>
+  <si>
+    <t>nClerks = 4</t>
+  </si>
+  <si>
+    <t>Theoretically</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  75 nClerks=4 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  80 nClerks=4 nInBank=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  85 nClerks=4 nInBank=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  90 nClerks=4 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec  95 nClerks=4 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 100 nClerks=4 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 105 nClerks=5 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 110 nClerks=5 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 115 nClerks=5 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 120 nClerks=5 nInBank=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 125 nClerks=5 nInBank=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 130 nClerks=5 nInBank=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 135 nClerks=5 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 140 nClerks=5 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 145 nClerks=5 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 150 nClerks=6 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 155 nClerks=6 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 160 nClerks=6 nInBank=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 165 nClerks=6 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 170 nClerks=6 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 175 nClerks=6 nInBank=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sec 180 nClerks=6 nInBank=4</t>
+  </si>
+  <si>
+    <t>Sums</t>
+  </si>
+  <si>
+    <t>numNLine</t>
+  </si>
+  <si>
+    <t>numNBank</t>
+  </si>
+  <si>
+    <t>Wait time</t>
+  </si>
+  <si>
+    <t>3, 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +314,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,8 +357,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -161,11 +384,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -176,12 +414,65 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -490,10 +781,887 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B8E858-8925-4990-9657-6B578BFB9E4C}">
+  <dimension ref="A1:AI38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="11"/>
+    <col min="5" max="6" width="19" style="11" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="13" style="11" customWidth="1"/>
+    <col min="10" max="14" width="9.140625" style="11"/>
+    <col min="15" max="35" width="9.140625" style="17"/>
+    <col min="36" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" s="8" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+    </row>
+    <row r="2" spans="1:35" s="10" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6">
+        <f>COUNT(E3:E198)</f>
+        <v>22</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="16"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="16"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11">
+        <v>15</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11">
+        <f>COUNT(E3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C4" s="11">
+        <f>C3+15</f>
+        <v>30</v>
+      </c>
+      <c r="D4" s="11">
+        <v>2</v>
+      </c>
+      <c r="E4" s="11">
+        <f>E3+1</f>
+        <v>2</v>
+      </c>
+      <c r="G4" s="11">
+        <f>COUNT(E3:E4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C5" s="11">
+        <f t="shared" ref="C5:C38" si="0">C4+15</f>
+        <v>45</v>
+      </c>
+      <c r="D5" s="11">
+        <v>3</v>
+      </c>
+      <c r="E5" s="11">
+        <v>3</v>
+      </c>
+      <c r="G5" s="11">
+        <f>COUNT(E3:E5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D6" s="11">
+        <v>4</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" ref="E6:E25" si="1">E5+1</f>
+        <v>4</v>
+      </c>
+      <c r="G6" s="11">
+        <f>COUNT(E3:E6)</f>
+        <v>4</v>
+      </c>
+      <c r="H6" s="11">
+        <v>1</v>
+      </c>
+      <c r="I6" s="11">
+        <v>3</v>
+      </c>
+      <c r="J6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="12">
+        <f>C6+15</f>
+        <v>75</v>
+      </c>
+      <c r="D7" s="12">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F7" s="11">
+        <f>E7*15-C7</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="19">
+        <f>COUNT(E3:E7)</f>
+        <v>5</v>
+      </c>
+      <c r="H7" s="13">
+        <v>1</v>
+      </c>
+      <c r="I7" s="13">
+        <v>4</v>
+      </c>
+      <c r="M7" s="12">
+        <v>4</v>
+      </c>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="18"/>
+      <c r="AG7" s="18"/>
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="18"/>
+    </row>
+    <row r="8" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="14">
+        <v>80</v>
+      </c>
+      <c r="D8" s="14">
+        <v>5</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="5">
+        <f>COUNT(E3:E7)</f>
+        <v>5</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5">
+        <v>4</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C9" s="11">
+        <f>C7+15</f>
+        <v>90</v>
+      </c>
+      <c r="D9" s="11">
+        <v>6</v>
+      </c>
+      <c r="E9" s="11">
+        <f>E7+1</f>
+        <v>6</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C10" s="11">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="D10" s="11">
+        <v>7</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="11">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="D11" s="11">
+        <v>8</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J11" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K11" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C12" s="14">
+        <v>125</v>
+      </c>
+      <c r="D12" s="11">
+        <v>9</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C13" s="11">
+        <f>C11+15</f>
+        <v>135</v>
+      </c>
+      <c r="D13" s="11">
+        <v>10</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C14" s="11">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="D14" s="11">
+        <v>11</v>
+      </c>
+      <c r="E14" s="11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C15" s="11">
+        <v>160</v>
+      </c>
+      <c r="D15" s="11">
+        <v>12</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="L15" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C16" s="11">
+        <f>C14+15</f>
+        <v>165</v>
+      </c>
+      <c r="D16" s="11">
+        <v>13</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="11">
+        <v>3</v>
+      </c>
+      <c r="C17" s="11">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="D17" s="11">
+        <v>14</v>
+      </c>
+      <c r="E17" s="11">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J17" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C18" s="11">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="D18" s="11">
+        <v>15</v>
+      </c>
+      <c r="E18" s="11">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C19" s="11">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="D19" s="11">
+        <v>16</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C20" s="11">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="D20" s="11">
+        <v>17</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
+        <v>4</v>
+      </c>
+      <c r="C21" s="11">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="D21" s="11">
+        <v>18</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J21" s="11">
+        <v>-1</v>
+      </c>
+      <c r="L21" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C22" s="11">
+        <f t="shared" si="0"/>
+        <v>255</v>
+      </c>
+      <c r="D22" s="11">
+        <v>19</v>
+      </c>
+      <c r="E22" s="11">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C23" s="11">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="D23" s="11">
+        <v>20</v>
+      </c>
+      <c r="E23" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C24" s="11">
+        <f t="shared" si="0"/>
+        <v>285</v>
+      </c>
+      <c r="D24" s="11">
+        <v>21</v>
+      </c>
+      <c r="E24" s="11">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <v>5</v>
+      </c>
+      <c r="C25" s="11">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="D25" s="11">
+        <v>22</v>
+      </c>
+      <c r="E25" s="11">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J25" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C26" s="11">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C27" s="14">
+        <v>320</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="L27" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C28" s="11">
+        <f>C26+15</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C29" s="11">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C30" s="11">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C31" s="11">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C32" s="11">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="11">
+        <f t="shared" si="0"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="11">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="11">
+        <f t="shared" si="0"/>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="11">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="11">
+        <f t="shared" si="0"/>
+        <v>465</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="11">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B03BBB-29F0-498C-98F8-D74F0474822E}">
+  <dimension ref="B1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="39.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63444096-9F63-48D8-85CB-C95C2BD4FB84}">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>

</xml_diff>